<commit_message>
Update on CorrosionEvolution figures
</commit_message>
<xml_diff>
--- a/VAC Prelim 2.0/Chapter-4/figs/dcvsicor_2020_01.xlsx
+++ b/VAC Prelim 2.0/Chapter-4/figs/dcvsicor_2020_01.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ConditionDependent_PBD\Thesis\VAC Thesis 1.0\Chapter-4\figs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ConditionDepedentPBEE\Thesis\VAC Prelim 2.0\Chapter-4\figs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD1C171C-6277-4B5F-A0B2-79D249D53FA8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="23235" windowHeight="12555" activeTab="3"/>
+    <workbookView xWindow="732" yWindow="540" windowWidth="20748" windowHeight="11082" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +19,7 @@
     <sheet name="Strain Aging" sheetId="8" r:id="rId4"/>
     <sheet name="Time to Corrosion" sheetId="6" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +27,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -267,7 +271,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -663,7 +667,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -821,7 +824,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1020,80 +1022,86 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet2!$C$50:$C$73</c:f>
+              <c:f>Sheet2!$C$50:$C$75</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="24"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.778</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>5.5</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>6.5</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>7.5</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>8.5</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>9.5</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="13">
                   <c:v>15</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="14">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="15">
                   <c:v>25</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="16">
                   <c:v>30</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="17">
                   <c:v>35</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="18">
                   <c:v>40</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="19">
                   <c:v>45</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="20">
                   <c:v>50</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="21">
                   <c:v>55</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="22">
                   <c:v>60</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="23">
                   <c:v>65</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="24">
                   <c:v>70</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="25">
                   <c:v>75</c:v>
                 </c:pt>
               </c:numCache>
@@ -1101,80 +1109,86 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet2!$D$50:$D$73</c:f>
+              <c:f>Sheet2!$D$50:$D$75</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="24"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>0.74506530483898725</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>0.74453308375157368</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>0.74402126724230888</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>0.74352677583696258</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>0.74304726983538649</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>0.74258091793826897</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>0.74212625213420225</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>0.74168207232912142</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>0.74124738123333467</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>0.74082133847659459</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
                   <c:v>0.74040322739662956</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="13">
                   <c:v>0.73655340955618331</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="14">
                   <c:v>0.7331144819703318</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="15">
                   <c:v>0.72994235550458131</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="16">
                   <c:v>0.72696392265787313</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="17">
                   <c:v>0.72413553507543715</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="18">
                   <c:v>0.72142845544552847</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="19">
                   <c:v>0.71882247409659372</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="20">
                   <c:v>0.71630268450143153</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="21">
                   <c:v>0.7138576868735701</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="22">
                   <c:v>0.71147851205598589</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="23">
                   <c:v>0.7091579396763229</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="24">
                   <c:v>0.70689004631766394</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="25">
                   <c:v>0.70466989493238885</c:v>
                 </c:pt>
               </c:numCache>
@@ -1219,80 +1233,86 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet2!$C$50:$C$73</c:f>
+              <c:f>Sheet2!$C$50:$C$75</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="24"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.778</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>5.5</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>6.5</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>7.5</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>8.5</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>9.5</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="13">
                   <c:v>15</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="14">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="15">
                   <c:v>25</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="16">
                   <c:v>30</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="17">
                   <c:v>35</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="18">
                   <c:v>40</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="19">
                   <c:v>45</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="20">
                   <c:v>50</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="21">
                   <c:v>55</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="22">
                   <c:v>60</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="23">
                   <c:v>65</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="24">
                   <c:v>70</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="25">
                   <c:v>75</c:v>
                 </c:pt>
               </c:numCache>
@@ -1300,80 +1320,86 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet2!$E$50:$E$73</c:f>
+              <c:f>Sheet2!$E$50:$E$75</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="24"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>0.74451435832114665</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>0.74392271606479266</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>0.74335375650730473</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>0.74280405635876601</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>0.7422710146972894</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>0.74175259576352193</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>0.74124716764621013</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>0.74075339626375314</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>0.74027017298153031</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>0.73979656360403279</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
                   <c:v>0.73933177145541795</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="13">
                   <c:v>0.73505213096852517</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="14">
                   <c:v>0.73122925561757168</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="15">
                   <c:v>0.72770296907233667</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="16">
                   <c:v>0.72439200155996564</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="17">
                   <c:v>0.7212478314947619</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="18">
                   <c:v>0.71823851311515308</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="19">
                   <c:v>0.71534158038970852</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="20">
                   <c:v>0.71254046251430836</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="21">
                   <c:v>0.70982248694449812</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="22">
                   <c:v>0.70717768313904084</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="23">
                   <c:v>0.70459802458885346</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="24">
                   <c:v>0.70207692654216047</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="25">
                   <c:v>0.69960890074217796</c:v>
                 </c:pt>
               </c:numCache>
@@ -1416,80 +1442,86 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet2!$C$50:$C$73</c:f>
+              <c:f>Sheet2!$C$50:$C$75</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="24"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.778</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>5.5</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>6.5</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>7.5</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>8.5</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>9.5</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="13">
                   <c:v>15</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="14">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="15">
                   <c:v>25</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="16">
                   <c:v>30</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="17">
                   <c:v>35</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="18">
                   <c:v>40</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="19">
                   <c:v>45</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="20">
                   <c:v>50</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="21">
                   <c:v>55</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="22">
                   <c:v>60</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="23">
                   <c:v>65</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="24">
                   <c:v>70</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="25">
                   <c:v>75</c:v>
                 </c:pt>
               </c:numCache>
@@ -1497,80 +1529,86 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet2!$F$50:$F$73</c:f>
+              <c:f>Sheet2!$F$50:$F$75</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="24"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>0.7436729586027887</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>0.7429905689631735</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>0.74233434114438568</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>0.7417003267848139</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>0.7410855260274839</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>0.74048759086382021</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>0.73990463907645254</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>0.73933513195942635</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>0.73877779083331774</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>0.73823153821366783</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
                   <c:v>0.7376954552287508</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="13">
                   <c:v>0.73275939412396995</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="14">
                   <c:v>0.72835015779067047</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="15">
                   <c:v>0.7242830017027807</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="16">
                   <c:v>0.7204641907519399</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="17">
                   <c:v>0.71683776100551588</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="18">
                   <c:v>0.71336686679115779</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="19">
                   <c:v>0.71002559618839844</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="20">
                   <c:v>0.70679483672694032</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="21">
                   <c:v>0.70365997211974385</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="22">
                   <c:v>0.70060950252215104</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="23">
                   <c:v>0.6976341703015605</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="24">
                   <c:v>0.69472638072256843</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="25">
                   <c:v>0.69187980372756153</c:v>
                 </c:pt>
               </c:numCache>
@@ -1587,7 +1625,7 @@
           <c:idx val="3"/>
           <c:order val="3"/>
           <c:tx>
-            <c:v>w/c=0.5</c:v>
+            <c:v>w/c=0.50</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -1615,80 +1653,86 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet2!$C$50:$C$73</c:f>
+              <c:f>Sheet2!$C$50:$C$75</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="24"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.778</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>5.5</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>6.5</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>7.5</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>8.5</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>9.5</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="13">
                   <c:v>15</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="14">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="15">
                   <c:v>25</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="16">
                   <c:v>30</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="17">
                   <c:v>35</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="18">
                   <c:v>40</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="19">
                   <c:v>45</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="20">
                   <c:v>50</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="21">
                   <c:v>55</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="22">
                   <c:v>60</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="23">
                   <c:v>65</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="24">
                   <c:v>70</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="25">
                   <c:v>75</c:v>
                 </c:pt>
               </c:numCache>
@@ -1696,80 +1740,86 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet2!$G$50:$G$73</c:f>
+              <c:f>Sheet2!$G$50:$G$75</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="24"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>0.74260250501051028</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>0.74180466386754618</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>0.74103741078720653</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>0.74029612939615019</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>0.73957731230039236</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>0.73887821423866773</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>0.73819663454676498</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>0.73753077418957869</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>0.73687913815166017</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>0.73624046665211285</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
                   <c:v>0.73561368535799609</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="13">
                   <c:v>0.72984250654027494</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="14">
                   <c:v>0.72468728443323538</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="15">
                   <c:v>0.71993201812584295</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="16">
                   <c:v>0.71546711374144867</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="17">
                   <c:v>0.71122713897366363</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="18">
                   <c:v>0.70716901433880996</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="19">
                   <c:v>0.70326244395453297</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="20">
                   <c:v>0.69948508176769519</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="21">
                   <c:v>0.69581983860448704</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="22">
                   <c:v>0.69225326899523332</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="23">
                   <c:v>0.68877454903560342</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="24">
                   <c:v>0.68537479905916643</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="25">
                   <c:v>0.6820466180444128</c:v>
                 </c:pt>
               </c:numCache>
@@ -1836,12 +1886,11 @@
                       <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
                   </a:rPr>
-                  <a:t>Time (Years)</a:t>
+                  <a:t>Time, t (Years)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1909,7 +1958,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.75000000000000011"/>
-          <c:min val="0.60000000000000009"/>
+          <c:min val="0.67500000000000016"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1949,12 +1998,27 @@
                       <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
                   </a:rPr>
-                  <a:t>Diameter (in)</a:t>
+                  <a:t>Bar diameter, d</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" baseline="-25000">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>b</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t> (in)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2015,8 +2079,8 @@
         <c:crossAx val="480087864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="5.000000000000001E-2"/>
-        <c:minorUnit val="2.5000000000000005E-2"/>
+        <c:majorUnit val="2.5000000000000005E-2"/>
+        <c:minorUnit val="5.000000000000001E-3"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -3004,7 +3068,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3134,7 +3197,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3642,7 +3704,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3763,7 +3824,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3886,7 +3946,6 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -3894,6 +3953,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -4315,12 +4375,11 @@
                       <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
                   </a:rPr>
-                  <a:t>Time (Days)</a:t>
+                  <a:t>Time, t (Days)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4425,7 +4484,7 @@
                       <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
                   </a:rPr>
-                  <a:t>F</a:t>
+                  <a:t>Level of strain aging, F</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-US" sz="1400" baseline="-25000">
@@ -4454,7 +4513,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4569,7 +4627,6 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -4577,6 +4634,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -7411,7 +7469,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7482,7 +7540,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7523,7 +7581,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7579,19 +7637,25 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>390525</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>158115</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>116205</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>144780</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 1"/>
+        <xdr:cNvPr id="3" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -7621,7 +7685,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 1"/>
+        <xdr:cNvPr id="4" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -7659,7 +7729,7 @@
         <xdr:cNvPr id="2" name="Picture 1" descr="VictorCalderon-thesis.pdf - Adobe Acrobat Pro DC">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C671BCD8-262D-4460-9B29-F293E3BCD792}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7708,7 +7778,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E670BEE-2C24-4410-AE4C-497E1B3667D2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7749,7 +7819,7 @@
         <xdr:cNvPr id="2" name="Picture 1" descr="VictorCalderon-thesis.pdf - Adobe Acrobat Pro DC">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0BB292F-02AC-434B-A2D6-C79985EE17EF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7798,7 +7868,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B65E973F-5F2A-44C6-BFCF-AE35698BEA17}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7839,7 +7909,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A7A1AE99-2CF2-499E-925E-A85203F44D60}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8157,16 +8227,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:H18"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="D3">
         <v>40</v>
       </c>
@@ -8177,7 +8247,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -8191,7 +8261,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C5">
         <v>0.36</v>
       </c>
@@ -8208,7 +8278,7 @@
         <v>1.0395247813877899</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C6">
         <v>0.4</v>
       </c>
@@ -8225,7 +8295,7 @@
         <v>1.1555851538783679</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C7">
         <v>0.42</v>
       </c>
@@ -8242,7 +8312,7 @@
         <v>1.2216536443727766</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C8">
         <v>0.5</v>
       </c>
@@ -8259,12 +8329,12 @@
         <v>1.5583291593209996</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="D10" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C11" t="s">
         <v>0</v>
       </c>
@@ -8284,7 +8354,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C12">
         <v>40</v>
       </c>
@@ -8293,23 +8363,23 @@
         <v>1.5748031496062993</v>
       </c>
       <c r="E12">
-        <f>37.5*((1-E$11)^(-1.64))/$C12</f>
+        <f t="shared" ref="E12:H18" si="5">37.5*((1-E$11)^(-1.64))/$C12</f>
         <v>1.9491089651021061</v>
       </c>
       <c r="F12">
-        <f>37.5*((1-F$11)^(-1.64))/$C12</f>
+        <f t="shared" si="5"/>
         <v>2.16672216352194</v>
       </c>
       <c r="G12">
-        <f>37.5*((1-G$11)^(-1.64))/$C12</f>
+        <f t="shared" si="5"/>
         <v>2.2906005831989562</v>
       </c>
       <c r="H12">
-        <f>37.5*((1-H$11)^(-1.64))/$C12</f>
+        <f t="shared" si="5"/>
         <v>2.9218671737268744</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C13">
         <v>50</v>
       </c>
@@ -8318,23 +8388,23 @@
         <v>1.9685039370078741</v>
       </c>
       <c r="E13">
-        <f>37.5*((1-E$11)^(-1.64))/$C13</f>
+        <f t="shared" si="5"/>
         <v>1.5592871720816848</v>
       </c>
       <c r="F13">
-        <f>37.5*((1-F$11)^(-1.64))/$C13</f>
+        <f t="shared" si="5"/>
         <v>1.733377730817552</v>
       </c>
       <c r="G13">
-        <f>37.5*((1-G$11)^(-1.64))/$C13</f>
+        <f t="shared" si="5"/>
         <v>1.8324804665591647</v>
       </c>
       <c r="H13">
-        <f>37.5*((1-H$11)^(-1.64))/$C13</f>
+        <f t="shared" si="5"/>
         <v>2.3374937389814994</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C14">
         <v>60</v>
       </c>
@@ -8343,23 +8413,23 @@
         <v>2.3622047244094491</v>
       </c>
       <c r="E14">
-        <f>37.5*((1-E$11)^(-1.64))/$C14</f>
+        <f t="shared" si="5"/>
         <v>1.2994059767347372</v>
       </c>
       <c r="F14">
-        <f>37.5*((1-F$11)^(-1.64))/$C14</f>
+        <f t="shared" si="5"/>
         <v>1.4444814423479599</v>
       </c>
       <c r="G14">
-        <f>37.5*((1-G$11)^(-1.64))/$C14</f>
+        <f t="shared" si="5"/>
         <v>1.5270670554659707</v>
       </c>
       <c r="H14">
-        <f>37.5*((1-H$11)^(-1.64))/$C14</f>
+        <f t="shared" si="5"/>
         <v>1.9479114491512495</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C15">
         <v>70</v>
       </c>
@@ -8368,23 +8438,23 @@
         <v>2.7559055118110236</v>
       </c>
       <c r="E15">
-        <f>37.5*((1-E$11)^(-1.64))/$C15</f>
+        <f t="shared" si="5"/>
         <v>1.1137765514869178</v>
       </c>
       <c r="F15">
-        <f>37.5*((1-F$11)^(-1.64))/$C15</f>
+        <f t="shared" si="5"/>
         <v>1.2381269505839656</v>
       </c>
       <c r="G15">
-        <f>37.5*((1-G$11)^(-1.64))/$C15</f>
+        <f t="shared" si="5"/>
         <v>1.3089146189708321</v>
       </c>
       <c r="H15">
-        <f>37.5*((1-H$11)^(-1.64))/$C15</f>
+        <f t="shared" si="5"/>
         <v>1.6696383849867853</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C16">
         <v>80</v>
       </c>
@@ -8393,23 +8463,23 @@
         <v>3.1496062992125986</v>
       </c>
       <c r="E16">
-        <f>37.5*((1-E$11)^(-1.64))/$C16</f>
+        <f t="shared" si="5"/>
         <v>0.97455448255105304</v>
       </c>
       <c r="F16">
-        <f>37.5*((1-F$11)^(-1.64))/$C16</f>
+        <f t="shared" si="5"/>
         <v>1.08336108176097</v>
       </c>
       <c r="G16">
-        <f>37.5*((1-G$11)^(-1.64))/$C16</f>
+        <f t="shared" si="5"/>
         <v>1.1453002915994781</v>
       </c>
       <c r="H16">
-        <f>37.5*((1-H$11)^(-1.64))/$C16</f>
+        <f t="shared" si="5"/>
         <v>1.4609335868634372</v>
       </c>
     </row>
-    <row r="17" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C17">
         <v>90</v>
       </c>
@@ -8418,23 +8488,23 @@
         <v>3.5433070866141736</v>
       </c>
       <c r="E17">
-        <f>37.5*((1-E$11)^(-1.64))/$C17</f>
+        <f t="shared" si="5"/>
         <v>0.8662706511564916</v>
       </c>
       <c r="F17">
-        <f>37.5*((1-F$11)^(-1.64))/$C17</f>
+        <f t="shared" si="5"/>
         <v>0.96298762823197326</v>
       </c>
       <c r="G17">
-        <f>37.5*((1-G$11)^(-1.64))/$C17</f>
+        <f t="shared" si="5"/>
         <v>1.0180447036439804</v>
       </c>
       <c r="H17">
-        <f>37.5*((1-H$11)^(-1.64))/$C17</f>
+        <f t="shared" si="5"/>
         <v>1.2986076327674996</v>
       </c>
     </row>
-    <row r="18" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C18">
         <v>100</v>
       </c>
@@ -8443,19 +8513,19 @@
         <v>3.9370078740157481</v>
       </c>
       <c r="E18">
-        <f>37.5*((1-E$11)^(-1.64))/$C18</f>
+        <f t="shared" si="5"/>
         <v>0.77964358604084238</v>
       </c>
       <c r="F18">
-        <f>37.5*((1-F$11)^(-1.64))/$C18</f>
+        <f t="shared" si="5"/>
         <v>0.86668886540877599</v>
       </c>
       <c r="G18">
-        <f>37.5*((1-G$11)^(-1.64))/$C18</f>
+        <f t="shared" si="5"/>
         <v>0.91624023327958237</v>
       </c>
       <c r="H18">
-        <f>37.5*((1-H$11)^(-1.64))/$C18</f>
+        <f t="shared" si="5"/>
         <v>1.1687468694907497</v>
       </c>
     </row>
@@ -8466,36 +8536,36 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V78"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:V80"/>
   <sheetViews>
-    <sheetView topLeftCell="L17" workbookViewId="0">
-      <selection activeCell="AC47" sqref="AC47"/>
+    <sheetView topLeftCell="H44" workbookViewId="0">
+      <selection activeCell="I67" sqref="I67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B14" t="s">
         <v>3</v>
       </c>
@@ -8511,7 +8581,7 @@
         <v>2.2231790645402709</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" t="s">
         <v>0</v>
       </c>
@@ -8526,7 +8596,7 @@
         <v>2.2231790645402709</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B16" t="s">
         <v>5</v>
       </c>
@@ -8534,7 +8604,7 @@
         <v>1.778</v>
       </c>
     </row>
-    <row r="17" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:22" x14ac:dyDescent="0.55000000000000004">
       <c r="D17">
         <v>0.36</v>
       </c>
@@ -8548,7 +8618,7 @@
         <v>0.5</v>
       </c>
       <c r="H17">
-        <v>0.8</v>
+        <v>0.6</v>
       </c>
       <c r="L17">
         <v>0.36</v>
@@ -8566,7 +8636,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="18" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:22" x14ac:dyDescent="0.55000000000000004">
       <c r="C18" t="s">
         <v>4</v>
       </c>
@@ -8580,7 +8650,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:22" x14ac:dyDescent="0.55000000000000004">
       <c r="C19">
         <v>5</v>
       </c>
@@ -8602,7 +8672,7 @@
       </c>
       <c r="H19">
         <f t="shared" si="0"/>
-        <v>18.205615970584759</v>
+        <v>18.779073917289988</v>
       </c>
       <c r="J19">
         <f>+(C19-$C$16)^0.71</f>
@@ -8629,7 +8699,7 @@
       </c>
       <c r="P19" s="1">
         <f t="shared" si="1"/>
-        <v>8.668456990951863E-2</v>
+        <v>2.8241422445309212E-2</v>
       </c>
       <c r="R19">
         <f>(0.25*PI()*D19^2)/(1000^2)</f>
@@ -8652,7 +8722,7 @@
         <v>1.3115896044776987</v>
       </c>
     </row>
-    <row r="20" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:22" x14ac:dyDescent="0.55000000000000004">
       <c r="C20">
         <v>5.5</v>
       </c>
@@ -8674,7 +8744,7 @@
       </c>
       <c r="H20">
         <f t="shared" si="2"/>
-        <v>18.11454672077971</v>
+        <v>18.749853758872135</v>
       </c>
       <c r="J20">
         <f t="shared" ref="J20:J37" si="3">+(C20-$C$16)^0.71</f>
@@ -8701,7 +8771,7 @@
       </c>
       <c r="P20" s="1">
         <f t="shared" si="1"/>
-        <v>9.5799001386568106E-2</v>
+        <v>3.1263174050629033E-2</v>
       </c>
       <c r="R20">
         <f t="shared" ref="R20:R42" si="5">(0.25*PI()*D20^2)/(1000^2)</f>
@@ -8724,7 +8794,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="21" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:22" x14ac:dyDescent="0.55000000000000004">
       <c r="C21">
         <v>6</v>
       </c>
@@ -8746,7 +8816,7 @@
       </c>
       <c r="H21">
         <f t="shared" si="2"/>
-        <v>18.026968932828677</v>
+        <v>18.721753858595225</v>
       </c>
       <c r="J21">
         <f t="shared" si="3"/>
@@ -8773,7 +8843,7 @@
       </c>
       <c r="P21" s="1">
         <f t="shared" si="1"/>
-        <v>0.10452088672530398</v>
+        <v>3.4164637769579211E-2</v>
       </c>
       <c r="R21">
         <f t="shared" si="5"/>
@@ -8796,7 +8866,7 @@
         <v>-546.96888961601587</v>
       </c>
     </row>
-    <row r="22" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:22" x14ac:dyDescent="0.55000000000000004">
       <c r="C22">
         <v>6.5</v>
       </c>
@@ -8818,7 +8888,7 @@
       </c>
       <c r="H22">
         <f t="shared" si="2"/>
-        <v>17.942355672691281</v>
+        <v>18.694605146260834</v>
       </c>
       <c r="J22">
         <f t="shared" si="3"/>
@@ -8845,7 +8915,7 @@
       </c>
       <c r="P22" s="1">
         <f t="shared" si="1"/>
-        <v>0.11290738673512284</v>
+        <v>3.6963753144158146E-2</v>
       </c>
       <c r="R22">
         <f t="shared" si="5"/>
@@ -8868,7 +8938,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="23" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:22" x14ac:dyDescent="0.55000000000000004">
       <c r="C23">
         <v>7</v>
       </c>
@@ -8890,7 +8960,7 @@
       </c>
       <c r="H23">
         <f t="shared" si="2"/>
-        <v>17.860306590320707</v>
+        <v>18.668279166964417</v>
       </c>
       <c r="J23">
         <f t="shared" si="3"/>
@@ -8917,7 +8987,7 @@
       </c>
       <c r="P23" s="1">
         <f t="shared" si="1"/>
-        <v>0.12100205564785775</v>
+        <v>3.9674163017015131E-2</v>
       </c>
       <c r="R23">
         <f t="shared" si="5"/>
@@ -8940,7 +9010,7 @@
         <v>-14971.999423100038</v>
       </c>
     </row>
-    <row r="24" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:22" x14ac:dyDescent="0.55000000000000004">
       <c r="C24">
         <v>7.5</v>
       </c>
@@ -8962,7 +9032,7 @@
       </c>
       <c r="H24">
         <f t="shared" si="2"/>
-        <v>17.780508328996554</v>
+        <v>18.64267537817344</v>
       </c>
       <c r="J24">
         <f t="shared" si="3"/>
@@ -8989,7 +9059,7 @@
       </c>
       <c r="P24" s="1">
         <f t="shared" si="1"/>
-        <v>0.1288390781614458</v>
+        <v>4.2306555463370171E-2</v>
       </c>
       <c r="R24">
         <f t="shared" si="5"/>
@@ -9012,7 +9082,7 @@
         <v>-13412.515745234256</v>
       </c>
     </row>
-    <row r="25" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:22" x14ac:dyDescent="0.55000000000000004">
       <c r="C25">
         <v>8</v>
       </c>
@@ -9034,7 +9104,7 @@
       </c>
       <c r="H25">
         <f t="shared" si="2"/>
-        <v>17.702709694805645</v>
+        <v>18.61771318269453</v>
       </c>
       <c r="J25">
         <f t="shared" si="3"/>
@@ -9061,7 +9131,7 @@
       </c>
       <c r="P25" s="1">
         <f t="shared" si="1"/>
-        <v>0.13644593096336963</v>
+        <v>4.4869505850530865E-2</v>
       </c>
       <c r="R25">
         <f t="shared" si="5"/>
@@ -9084,7 +9154,7 @@
         <v>-12245.000883598344</v>
       </c>
     </row>
-    <row r="26" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:22" x14ac:dyDescent="0.55000000000000004">
       <c r="C26">
         <v>8.5</v>
       </c>
@@ -9106,7 +9176,7 @@
       </c>
       <c r="H26">
         <f t="shared" si="2"/>
-        <v>17.626705337624227</v>
+        <v>18.593326692610969</v>
       </c>
       <c r="J26">
         <f t="shared" si="3"/>
@@ -9133,7 +9203,7 @@
       </c>
       <c r="P26" s="1">
         <f t="shared" si="1"/>
-        <v>0.14384513454872738</v>
+        <v>4.737003052291E-2</v>
       </c>
       <c r="R26">
         <f>(0.25*PI()*D26^2)/(1000^2)</f>
@@ -9156,7 +9226,7 @@
         <v>-11292.248825224218</v>
       </c>
     </row>
-    <row r="27" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:22" x14ac:dyDescent="0.55000000000000004">
       <c r="C27">
         <v>9</v>
       </c>
@@ -9178,7 +9248,7 @@
       </c>
       <c r="H27">
         <f t="shared" si="2"/>
-        <v>17.552324609527549</v>
+        <v>18.569461154431252</v>
       </c>
       <c r="J27">
         <f t="shared" si="3"/>
@@ -9205,7 +9275,7 @@
       </c>
       <c r="P27" s="1">
         <f t="shared" si="1"/>
-        <v>0.15105545098690024</v>
+        <v>4.9813965001808271E-2</v>
       </c>
       <c r="R27">
         <f t="shared" si="5"/>
@@ -9228,7 +9298,7 @@
         <v>-10497.708185560055</v>
       </c>
     </row>
-    <row r="28" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:22" x14ac:dyDescent="0.55000000000000004">
       <c r="C28">
         <v>9.5</v>
       </c>
@@ -9250,7 +9320,7 @@
       </c>
       <c r="H28">
         <f t="shared" si="2"/>
-        <v>17.479423713342182</v>
+        <v>18.546070429901292</v>
       </c>
       <c r="J28">
         <f t="shared" si="3"/>
@@ -9277,7 +9347,7 @@
       </c>
       <c r="P28" s="1">
         <f t="shared" si="1"/>
-        <v>0.15809272917505646</v>
+        <v>5.220623062431605E-2</v>
       </c>
       <c r="R28">
         <f t="shared" si="5"/>
@@ -9300,7 +9370,7 @@
         <v>-9823.4134285522323</v>
       </c>
     </row>
-    <row r="29" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:22" x14ac:dyDescent="0.55000000000000004">
       <c r="C29">
         <v>10</v>
       </c>
@@ -9322,7 +9392,7 @@
       </c>
       <c r="H29">
         <f t="shared" si="2"/>
-        <v>17.4078800197756</v>
+        <v>18.523115172618628</v>
       </c>
       <c r="J29">
         <f t="shared" si="3"/>
@@ -9349,7 +9419,7 @@
       </c>
       <c r="P29" s="1">
         <f t="shared" si="1"/>
-        <v>0.16497051747259225</v>
+        <v>5.4551027622861473E-2</v>
       </c>
       <c r="R29">
         <f t="shared" si="5"/>
@@ -9372,7 +9442,7 @@
         <v>-9242.8596757817468</v>
       </c>
     </row>
-    <row r="30" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:22" x14ac:dyDescent="0.55000000000000004">
       <c r="C30">
         <v>15</v>
       </c>
@@ -9394,7 +9464,7 @@
       </c>
       <c r="H30">
         <f t="shared" si="2"/>
-        <v>16.749131182296548</v>
+        <v>18.311751343116111</v>
       </c>
       <c r="J30">
         <f t="shared" si="3"/>
@@ -9421,7 +9491,7 @@
       </c>
       <c r="P30" s="1">
         <f t="shared" si="1"/>
-        <v>0.22697309783818356</v>
+        <v>7.6004609358946942E-2</v>
       </c>
       <c r="R30">
         <f t="shared" si="5"/>
@@ -9444,7 +9514,7 @@
         <v>-8655.043250879633</v>
       </c>
     </row>
-    <row r="31" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:22" x14ac:dyDescent="0.55000000000000004">
       <c r="C31">
         <v>20</v>
       </c>
@@ -9466,7 +9536,7 @@
       </c>
       <c r="H31">
         <f t="shared" si="2"/>
-        <v>16.160690470750644</v>
+        <v>18.12294633102152</v>
       </c>
       <c r="J31">
         <f t="shared" si="3"/>
@@ -9493,7 +9563,7 @@
       </c>
       <c r="P31" s="1">
         <f t="shared" si="1"/>
-        <v>0.2803358574509387</v>
+        <v>9.4960261455662318E-2</v>
       </c>
       <c r="R31">
         <f t="shared" si="5"/>
@@ -9516,7 +9586,7 @@
         <v>-8145.3283747705827</v>
       </c>
     </row>
-    <row r="32" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:22" x14ac:dyDescent="0.55000000000000004">
       <c r="C32">
         <v>25</v>
       </c>
@@ -9538,7 +9608,7 @@
       </c>
       <c r="H32">
         <f t="shared" si="2"/>
-        <v>15.617902549801242</v>
+        <v>17.948789312363825</v>
       </c>
       <c r="J32">
         <f t="shared" si="3"/>
@@ -9565,7 +9635,7 @@
       </c>
       <c r="P32" s="1">
         <f t="shared" si="1"/>
-        <v>0.32786663069257388</v>
+        <v>0.11227109821611617</v>
       </c>
       <c r="R32">
         <f t="shared" si="5"/>
@@ -9588,7 +9658,7 @@
         <v>-7697.1352630444799</v>
       </c>
     </row>
-    <row r="33" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:22" x14ac:dyDescent="0.55000000000000004">
       <c r="C33">
         <v>30</v>
       </c>
@@ -9610,7 +9680,7 @@
       </c>
       <c r="H33">
         <f t="shared" si="2"/>
-        <v>15.108257871378999</v>
+        <v>17.78526651765327</v>
       </c>
       <c r="J33">
         <f t="shared" si="3"/>
@@ -9637,7 +9707,7 @@
       </c>
       <c r="P33" s="1">
         <f t="shared" si="1"/>
-        <v>0.37101713019864685</v>
+        <v>0.12837275823683084</v>
       </c>
       <c r="R33">
         <f t="shared" si="5"/>
@@ -9660,7 +9730,7 @@
         <v>-7298.9560445767911</v>
       </c>
     </row>
-    <row r="34" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:22" x14ac:dyDescent="0.55000000000000004">
       <c r="C34">
         <v>35</v>
       </c>
@@ -9682,7 +9752,7 @@
       </c>
       <c r="H34">
         <f t="shared" si="2"/>
-        <v>14.624287691726565</v>
+        <v>17.629981552099743</v>
       </c>
       <c r="J34">
         <f t="shared" si="3"/>
@@ -9709,7 +9779,7 @@
       </c>
       <c r="P34" s="1">
         <f t="shared" si="1"/>
-        <v>0.41066873198618048</v>
+        <v>0.1435268439115816</v>
       </c>
       <c r="R34">
         <f t="shared" si="5"/>
@@ -9732,7 +9802,7 @@
         <v>-5180.0433973354629</v>
       </c>
     </row>
-    <row r="35" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:22" x14ac:dyDescent="0.55000000000000004">
       <c r="C35">
         <v>40</v>
       </c>
@@ -9754,7 +9824,7 @@
       </c>
       <c r="H35">
         <f t="shared" si="2"/>
-        <v>14.161074720860668</v>
+        <v>17.481356671375657</v>
       </c>
       <c r="J35">
         <f t="shared" si="3"/>
@@ -9781,7 +9851,7 @@
       </c>
       <c r="P35" s="1">
         <f t="shared" ref="P35:P47" si="13">($M$14-((0.25*PI()*H35^2)/(1000^2)*7800))/$M$15</f>
-        <v>0.44741070328862687</v>
+        <v>0.15790651463726421</v>
       </c>
       <c r="R35">
         <f t="shared" si="5"/>
@@ -9804,7 +9874,7 @@
         <v>-4081.7306086495009</v>
       </c>
     </row>
-    <row r="36" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:22" x14ac:dyDescent="0.55000000000000004">
       <c r="C36">
         <v>45</v>
       </c>
@@ -9826,7 +9896,7 @@
       </c>
       <c r="H36">
         <f t="shared" si="2"/>
-        <v>13.715160847724311</v>
+        <v>17.338282318159212</v>
       </c>
       <c r="J36">
         <f t="shared" si="3"/>
@@ -9853,7 +9923,7 @@
       </c>
       <c r="P36" s="1">
         <f t="shared" si="13"/>
-        <v>0.48166343004264256</v>
+        <v>0.17163416139543694</v>
       </c>
       <c r="R36">
         <f t="shared" si="5"/>
@@ -9876,7 +9946,7 @@
         <v>-3402.0650759563096</v>
       </c>
     </row>
-    <row r="37" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:22" x14ac:dyDescent="0.55000000000000004">
       <c r="C37">
         <v>50</v>
       </c>
@@ -9898,7 +9968,7 @@
       </c>
       <c r="H37">
         <f t="shared" si="2"/>
-        <v>13.283995391253629</v>
+        <v>17.199940089916961</v>
       </c>
       <c r="J37">
         <f t="shared" si="3"/>
@@ -9925,7 +9995,7 @@
       </c>
       <c r="P37" s="1">
         <f t="shared" si="13"/>
-        <v>0.51374120168682302</v>
+        <v>0.18480049297887813</v>
       </c>
       <c r="R37">
         <f t="shared" si="5"/>
@@ -9948,7 +10018,7 @@
         <v>-2933.9305908603419</v>
       </c>
     </row>
-    <row r="38" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:22" x14ac:dyDescent="0.55000000000000004">
       <c r="C38">
         <v>55</v>
       </c>
@@ -9970,7 +10040,7 @@
       </c>
       <c r="H38">
         <f t="shared" si="2"/>
-        <v>12.865627714718052</v>
+        <v>17.065704112224715</v>
       </c>
       <c r="K38">
         <v>55</v>
@@ -9993,7 +10063,7 @@
       </c>
       <c r="P38" s="1">
         <f t="shared" si="13"/>
-        <v>0.54388747254780201</v>
+        <v>0.19747519830807569</v>
       </c>
       <c r="R38">
         <f t="shared" si="5"/>
@@ -10016,7 +10086,7 @@
         <v>-2588.9344644622083</v>
       </c>
     </row>
-    <row r="39" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:22" x14ac:dyDescent="0.55000000000000004">
       <c r="C39">
         <v>60</v>
       </c>
@@ -10038,7 +10108,7 @@
       </c>
       <c r="H39">
         <f t="shared" si="2"/>
-        <v>12.458523090499927</v>
+        <v>16.935081957789926</v>
       </c>
       <c r="K39">
         <v>60</v>
@@ -10061,7 +10131,7 @@
       </c>
       <c r="P39" s="1">
         <f t="shared" si="13"/>
-        <v>0.57229614677077212</v>
+        <v>0.20971335023301868</v>
       </c>
       <c r="R39">
         <f t="shared" si="5"/>
@@ -10084,7 +10154,7 @@
         <v>-2322.5295764940424</v>
       </c>
     </row>
-    <row r="40" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:22" x14ac:dyDescent="0.55000000000000004">
       <c r="C40">
         <v>65</v>
       </c>
@@ -10106,7 +10176,7 @@
       </c>
       <c r="H40">
         <f t="shared" si="2"/>
-        <v>12.0614460284819</v>
+        <v>16.807677211609395</v>
       </c>
       <c r="K40">
         <v>65</v>
@@ -10129,7 +10199,7 @@
       </c>
       <c r="P40" s="1">
         <f t="shared" si="13"/>
-        <v>0.59912516365144419</v>
+        <v>0.22155947327545608</v>
       </c>
       <c r="R40">
         <f t="shared" si="5"/>
@@ -10152,7 +10222,7 @@
         <v>-2109.6472664969497</v>
       </c>
     </row>
-    <row r="41" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:22" x14ac:dyDescent="0.55000000000000004">
       <c r="C41">
         <v>70</v>
       </c>
@@ -10174,7 +10244,7 @@
       </c>
       <c r="H41">
         <f t="shared" si="2"/>
-        <v>11.67338296278373</v>
+        <v>16.683164664508222</v>
       </c>
       <c r="K41">
         <v>70</v>
@@ -10197,7 +10267,7 @@
       </c>
       <c r="P41" s="1">
         <f t="shared" si="13"/>
-        <v>0.62450556335156282</v>
+        <v>0.23305024566351612</v>
       </c>
       <c r="R41">
         <f t="shared" si="5"/>
@@ -10220,7 +10290,7 @@
         <v>-1935.0200060073348</v>
       </c>
     </row>
-    <row r="42" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:22" x14ac:dyDescent="0.55000000000000004">
       <c r="C42">
         <v>75</v>
       </c>
@@ -10242,7 +10312,7 @@
       </c>
       <c r="H42">
         <f t="shared" si="2"/>
-        <v>11.29348910684277</v>
+        <v>16.561273261248306</v>
       </c>
       <c r="K42">
         <v>75</v>
@@ -10265,7 +10335,7 @@
       </c>
       <c r="P42" s="1">
         <f t="shared" si="13"/>
-        <v>0.64854776088239585</v>
+        <v>0.24421636105086583</v>
       </c>
       <c r="R42">
         <f t="shared" si="5"/>
@@ -10288,7 +10358,7 @@
         <v>-1788.7783717720267</v>
       </c>
     </row>
-    <row r="43" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:22" x14ac:dyDescent="0.55000000000000004">
       <c r="C43">
         <v>80</v>
       </c>
@@ -10310,7 +10380,7 @@
       </c>
       <c r="H43">
         <f t="shared" si="2"/>
-        <v>10.921050787736258</v>
+        <v>16.441774015251784</v>
       </c>
       <c r="K43">
         <v>80</v>
@@ -10333,10 +10403,10 @@
       </c>
       <c r="P43" s="1">
         <f t="shared" si="13"/>
-        <v>0.67134602184246517</v>
-      </c>
-    </row>
-    <row r="44" spans="3:22" x14ac:dyDescent="0.25">
+        <v>0.25508385098309083</v>
+      </c>
+    </row>
+    <row r="44" spans="3:22" x14ac:dyDescent="0.55000000000000004">
       <c r="C44">
         <v>85</v>
       </c>
@@ -10358,7 +10428,7 @@
       </c>
       <c r="H44">
         <f t="shared" si="2"/>
-        <v>10.555458050723582</v>
+        <v>16.324471218591043</v>
       </c>
       <c r="K44">
         <v>85</v>
@@ -10381,10 +10451,10 @@
       </c>
       <c r="P44" s="1">
         <f t="shared" si="13"/>
-        <v>0.69298173845430855</v>
-      </c>
-    </row>
-    <row r="45" spans="3:22" x14ac:dyDescent="0.25">
+        <v>0.26567504889989074</v>
+      </c>
+    </row>
+    <row r="45" spans="3:22" x14ac:dyDescent="0.55000000000000004">
       <c r="C45">
         <v>90</v>
       </c>
@@ -10406,7 +10476,7 @@
       </c>
       <c r="H45">
         <f t="shared" si="2"/>
-        <v>10.196184285603914</v>
+        <v>16.209195904973662</v>
       </c>
       <c r="K45">
         <v>90</v>
@@ -10429,10 +10499,10 @@
       </c>
       <c r="P45" s="1">
         <f t="shared" si="13"/>
-        <v>0.71352588095701674</v>
-      </c>
-    </row>
-    <row r="46" spans="3:22" x14ac:dyDescent="0.25">
+        <v>0.27600930859992712</v>
+      </c>
+    </row>
+    <row r="46" spans="3:22" x14ac:dyDescent="0.55000000000000004">
       <c r="C46">
         <v>95</v>
       </c>
@@ -10454,7 +10524,7 @@
       </c>
       <c r="H46">
         <f t="shared" si="2"/>
-        <v>9.8427707797533994</v>
+        <v>16.095800893484402</v>
       </c>
       <c r="K46">
         <v>95</v>
@@ -10477,10 +10547,10 @@
       </c>
       <c r="P46" s="1">
         <f t="shared" si="13"/>
-        <v>0.73304086738788687</v>
-      </c>
-    </row>
-    <row r="47" spans="3:22" x14ac:dyDescent="0.25">
+        <v>0.28610355011967881</v>
+      </c>
+    </row>
+    <row r="47" spans="3:22" x14ac:dyDescent="0.55000000000000004">
       <c r="C47">
         <v>100</v>
       </c>
@@ -10502,7 +10572,7 @@
       </c>
       <c r="H47">
         <f t="shared" si="2"/>
-        <v>9.4948148066126556</v>
+        <v>15.984156966699267</v>
       </c>
       <c r="K47">
         <v>100</v>
@@ -10525,10 +10595,10 @@
       </c>
       <c r="P47" s="1">
         <f t="shared" si="13"/>
-        <v>0.75158201386909451</v>
-      </c>
-    </row>
-    <row r="49" spans="3:8" x14ac:dyDescent="0.25">
+        <v>0.29597268154371831</v>
+      </c>
+    </row>
+    <row r="49" spans="3:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C49" t="s">
         <v>50</v>
       </c>
@@ -10545,732 +10615,778 @@
         <v>0.5</v>
       </c>
       <c r="H49">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="50" spans="3:8" x14ac:dyDescent="0.25">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="50" spans="3:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="D50">
+        <v>0.75</v>
+      </c>
+      <c r="E50">
+        <v>0.75</v>
+      </c>
+      <c r="F50">
+        <v>0.75</v>
+      </c>
+      <c r="G50">
+        <v>0.75</v>
+      </c>
+      <c r="H50">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="51" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C51">
+        <f>+C16</f>
+        <v>1.778</v>
+      </c>
+      <c r="D51">
+        <f>+D50</f>
+        <v>0.75</v>
+      </c>
+      <c r="E51">
+        <f t="shared" ref="E51:H51" si="14">+E50</f>
+        <v>0.75</v>
+      </c>
+      <c r="F51">
+        <f t="shared" si="14"/>
+        <v>0.75</v>
+      </c>
+      <c r="G51">
+        <f t="shared" si="14"/>
+        <v>0.75</v>
+      </c>
+      <c r="H51">
+        <f t="shared" si="14"/>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="52" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C52">
         <v>5</v>
       </c>
-      <c r="D50">
+      <c r="D52">
         <f>+D19/25.4</f>
         <v>0.74506530483898725</v>
       </c>
-      <c r="E50">
-        <f t="shared" ref="E50:H50" si="14">+E19/25.4</f>
+      <c r="E52">
+        <f t="shared" ref="E52:H52" si="15">+E19/25.4</f>
         <v>0.74451435832114665</v>
       </c>
-      <c r="F50">
-        <f t="shared" si="14"/>
+      <c r="F52">
+        <f t="shared" si="15"/>
         <v>0.7436729586027887</v>
       </c>
-      <c r="G50">
-        <f t="shared" si="14"/>
+      <c r="G52">
+        <f t="shared" si="15"/>
         <v>0.74260250501051028</v>
       </c>
-      <c r="H50">
-        <f t="shared" si="14"/>
-        <v>0.71675653427499053</v>
-      </c>
-    </row>
-    <row r="51" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C51">
+      <c r="H52">
+        <f t="shared" si="15"/>
+        <v>0.7393336187909445</v>
+      </c>
+    </row>
+    <row r="53" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C53">
         <v>5.5</v>
       </c>
-      <c r="D51">
-        <f t="shared" ref="D51:H51" si="15">+D20/25.4</f>
+      <c r="D53">
+        <f t="shared" ref="D53:H53" si="16">+D20/25.4</f>
         <v>0.74453308375157368</v>
       </c>
-      <c r="E51">
-        <f t="shared" si="15"/>
+      <c r="E53">
+        <f t="shared" si="16"/>
         <v>0.74392271606479266</v>
       </c>
-      <c r="F51">
-        <f t="shared" si="15"/>
+      <c r="F53">
+        <f t="shared" si="16"/>
         <v>0.7429905689631735</v>
       </c>
-      <c r="G51">
-        <f t="shared" si="15"/>
+      <c r="G53">
+        <f t="shared" si="16"/>
         <v>0.74180466386754618</v>
       </c>
-      <c r="H51">
-        <f t="shared" si="15"/>
-        <v>0.71317113073935867</v>
-      </c>
-    </row>
-    <row r="52" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C52">
+      <c r="H53">
+        <f t="shared" si="16"/>
+        <v>0.73818321885323368</v>
+      </c>
+    </row>
+    <row r="54" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C54">
         <v>6</v>
       </c>
-      <c r="D52">
-        <f t="shared" ref="D52:H52" si="16">+D21/25.4</f>
+      <c r="D54">
+        <f t="shared" ref="D54:H54" si="17">+D21/25.4</f>
         <v>0.74402126724230888</v>
       </c>
-      <c r="E52">
-        <f t="shared" si="16"/>
+      <c r="E54">
+        <f t="shared" si="17"/>
         <v>0.74335375650730473</v>
       </c>
-      <c r="F52">
-        <f t="shared" si="16"/>
+      <c r="F54">
+        <f t="shared" si="17"/>
         <v>0.74233434114438568</v>
       </c>
-      <c r="G52">
-        <f t="shared" si="16"/>
+      <c r="G54">
+        <f t="shared" si="17"/>
         <v>0.74103741078720653</v>
       </c>
-      <c r="H52">
-        <f t="shared" si="16"/>
-        <v>0.70972318633183773</v>
-      </c>
-    </row>
-    <row r="53" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C53">
+      <c r="H54">
+        <f t="shared" si="17"/>
+        <v>0.73707692356674115</v>
+      </c>
+    </row>
+    <row r="55" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C55">
         <v>6.5</v>
       </c>
-      <c r="D53">
-        <f t="shared" ref="D53:H53" si="17">+D22/25.4</f>
+      <c r="D55">
+        <f t="shared" ref="D55:H55" si="18">+D22/25.4</f>
         <v>0.74352677583696258</v>
       </c>
-      <c r="E53">
-        <f t="shared" si="17"/>
+      <c r="E55">
+        <f t="shared" si="18"/>
         <v>0.74280405635876601</v>
       </c>
-      <c r="F53">
-        <f t="shared" si="17"/>
+      <c r="F55">
+        <f t="shared" si="18"/>
         <v>0.7417003267848139</v>
       </c>
-      <c r="G53">
-        <f t="shared" si="17"/>
+      <c r="G55">
+        <f t="shared" si="18"/>
         <v>0.74029612939615019</v>
       </c>
-      <c r="H53">
-        <f t="shared" si="17"/>
-        <v>0.70639195561776702</v>
-      </c>
-    </row>
-    <row r="54" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C54">
+      <c r="H55">
+        <f t="shared" si="18"/>
+        <v>0.73600807662444234</v>
+      </c>
+    </row>
+    <row r="56" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C56">
         <v>7</v>
       </c>
-      <c r="D54">
-        <f t="shared" ref="D54:H54" si="18">+D23/25.4</f>
+      <c r="D56">
+        <f t="shared" ref="D56:H56" si="19">+D23/25.4</f>
         <v>0.74304726983538649</v>
       </c>
-      <c r="E54">
-        <f t="shared" si="18"/>
+      <c r="E56">
+        <f t="shared" si="19"/>
         <v>0.7422710146972894</v>
       </c>
-      <c r="F54">
-        <f t="shared" si="18"/>
+      <c r="F56">
+        <f t="shared" si="19"/>
         <v>0.7410855260274839</v>
       </c>
-      <c r="G54">
-        <f t="shared" si="18"/>
+      <c r="G56">
+        <f t="shared" si="19"/>
         <v>0.73957731230039236</v>
       </c>
-      <c r="H54">
-        <f t="shared" si="18"/>
-        <v>0.70316167678427988</v>
-      </c>
-    </row>
-    <row r="55" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C55">
+      <c r="H56">
+        <f t="shared" si="19"/>
+        <v>0.73497162074663069</v>
+      </c>
+    </row>
+    <row r="57" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C57">
         <v>7.5</v>
       </c>
-      <c r="D55">
-        <f t="shared" ref="D55:H55" si="19">+D24/25.4</f>
+      <c r="D57">
+        <f t="shared" ref="D57:H57" si="20">+D24/25.4</f>
         <v>0.74258091793826897</v>
       </c>
-      <c r="E55">
-        <f t="shared" si="19"/>
+      <c r="E57">
+        <f t="shared" si="20"/>
         <v>0.74175259576352193</v>
       </c>
-      <c r="F55">
-        <f t="shared" si="19"/>
+      <c r="F57">
+        <f t="shared" si="20"/>
         <v>0.74048759086382021</v>
       </c>
-      <c r="G55">
-        <f t="shared" si="19"/>
+      <c r="G57">
+        <f t="shared" si="20"/>
         <v>0.73887821423866773</v>
       </c>
-      <c r="H55">
-        <f t="shared" si="19"/>
-        <v>0.70002001295262029</v>
-      </c>
-    </row>
-    <row r="56" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C56">
+      <c r="H57">
+        <f t="shared" si="20"/>
+        <v>0.73396359756588347</v>
+      </c>
+    </row>
+    <row r="58" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C58">
         <v>8</v>
       </c>
-      <c r="D56">
-        <f t="shared" ref="D56:H56" si="20">+D25/25.4</f>
+      <c r="D58">
+        <f t="shared" ref="D58:H58" si="21">+D25/25.4</f>
         <v>0.74212625213420225</v>
       </c>
-      <c r="E56">
-        <f t="shared" si="20"/>
+      <c r="E58">
+        <f t="shared" si="21"/>
         <v>0.74124716764621013</v>
       </c>
-      <c r="F56">
-        <f t="shared" si="20"/>
+      <c r="F58">
+        <f t="shared" si="21"/>
         <v>0.73990463907645254</v>
       </c>
-      <c r="G56">
-        <f t="shared" si="20"/>
+      <c r="G58">
+        <f t="shared" si="21"/>
         <v>0.73819663454676498</v>
       </c>
-      <c r="H56">
-        <f t="shared" si="20"/>
-        <v>0.69695707459864742</v>
-      </c>
-    </row>
-    <row r="57" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C57">
+      <c r="H58">
+        <f t="shared" si="21"/>
+        <v>0.73298083396435165</v>
+      </c>
+    </row>
+    <row r="59" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C59">
         <v>8.5</v>
       </c>
-      <c r="D57">
-        <f t="shared" ref="D57:H57" si="21">+D26/25.4</f>
+      <c r="D59">
+        <f t="shared" ref="D59:H59" si="22">+D26/25.4</f>
         <v>0.74168207232912142</v>
       </c>
-      <c r="E57">
-        <f t="shared" si="21"/>
+      <c r="E59">
+        <f t="shared" si="22"/>
         <v>0.74075339626375314</v>
       </c>
-      <c r="F57">
-        <f t="shared" si="21"/>
+      <c r="F59">
+        <f t="shared" si="22"/>
         <v>0.73933513195942635</v>
       </c>
-      <c r="G57">
-        <f t="shared" si="21"/>
+      <c r="G59">
+        <f t="shared" si="22"/>
         <v>0.73753077418957869</v>
       </c>
-      <c r="H57">
-        <f t="shared" si="21"/>
-        <v>0.69396477707182003</v>
-      </c>
-    </row>
-    <row r="58" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C58">
+      <c r="H59">
+        <f t="shared" si="22"/>
+        <v>0.73202073592956574</v>
+      </c>
+    </row>
+    <row r="60" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C60">
         <v>9</v>
       </c>
-      <c r="D58">
-        <f t="shared" ref="D58:H58" si="22">+D27/25.4</f>
+      <c r="D60">
+        <f t="shared" ref="D60:H60" si="23">+D27/25.4</f>
         <v>0.74124738123333467</v>
       </c>
-      <c r="E58">
-        <f t="shared" si="22"/>
+      <c r="E60">
+        <f t="shared" si="23"/>
         <v>0.74027017298153031</v>
       </c>
-      <c r="F58">
-        <f t="shared" si="22"/>
+      <c r="F60">
+        <f t="shared" si="23"/>
         <v>0.73877779083331774</v>
       </c>
-      <c r="G58">
-        <f t="shared" si="22"/>
+      <c r="G60">
+        <f t="shared" si="23"/>
         <v>0.73687913815166017</v>
       </c>
-      <c r="H58">
-        <f t="shared" si="22"/>
-        <v>0.69103640194990357</v>
-      </c>
-    </row>
-    <row r="59" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C59">
+      <c r="H60">
+        <f t="shared" si="23"/>
+        <v>0.73108114781225408</v>
+      </c>
+    </row>
+    <row r="61" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C61">
         <v>9.5</v>
       </c>
-      <c r="D59">
-        <f t="shared" ref="D59:H59" si="23">+D28/25.4</f>
+      <c r="D61">
+        <f t="shared" ref="D61:H61" si="24">+D28/25.4</f>
         <v>0.74082133847659459</v>
       </c>
-      <c r="E59">
-        <f t="shared" si="23"/>
+      <c r="E61">
+        <f t="shared" si="24"/>
         <v>0.73979656360403279</v>
       </c>
-      <c r="F59">
-        <f t="shared" si="23"/>
+      <c r="F61">
+        <f t="shared" si="24"/>
         <v>0.73823153821366783</v>
       </c>
-      <c r="G59">
-        <f t="shared" si="23"/>
+      <c r="G61">
+        <f t="shared" si="24"/>
         <v>0.73624046665211285</v>
       </c>
-      <c r="H59">
-        <f t="shared" si="23"/>
-        <v>0.68816628792685763</v>
-      </c>
-    </row>
-    <row r="60" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C60">
+      <c r="H61">
+        <f t="shared" si="24"/>
+        <v>0.7301602531457202</v>
+      </c>
+    </row>
+    <row r="62" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C62">
         <v>10</v>
       </c>
-      <c r="D60">
-        <f t="shared" ref="D60:H60" si="24">+D29/25.4</f>
+      <c r="D62">
+        <f t="shared" ref="D62:H62" si="25">+D29/25.4</f>
         <v>0.74040322739662956</v>
       </c>
-      <c r="E60">
-        <f t="shared" si="24"/>
+      <c r="E62">
+        <f t="shared" si="25"/>
         <v>0.73933177145541795</v>
       </c>
-      <c r="F60">
-        <f t="shared" si="24"/>
+      <c r="F62">
+        <f t="shared" si="25"/>
         <v>0.7376954552287508</v>
       </c>
-      <c r="G60">
-        <f t="shared" si="24"/>
+      <c r="G62">
+        <f t="shared" si="25"/>
         <v>0.73561368535799609</v>
       </c>
-      <c r="H60">
-        <f t="shared" si="24"/>
-        <v>0.68534960707777959</v>
-      </c>
-    </row>
-    <row r="61" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C61">
+      <c r="H62">
+        <f t="shared" si="25"/>
+        <v>0.72925650285900112</v>
+      </c>
+    </row>
+    <row r="63" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C63">
         <v>15</v>
       </c>
-      <c r="D61">
-        <f t="shared" ref="D61:H61" si="25">+D30/25.4</f>
+      <c r="D63">
+        <f t="shared" ref="D63:H63" si="26">+D30/25.4</f>
         <v>0.73655340955618331</v>
       </c>
-      <c r="E61">
-        <f t="shared" si="25"/>
+      <c r="E63">
+        <f t="shared" si="26"/>
         <v>0.73505213096852517</v>
       </c>
-      <c r="F61">
-        <f t="shared" si="25"/>
+      <c r="F63">
+        <f t="shared" si="26"/>
         <v>0.73275939412396995</v>
       </c>
-      <c r="G61">
-        <f t="shared" si="25"/>
+      <c r="G63">
+        <f t="shared" si="26"/>
         <v>0.72984250654027494</v>
       </c>
-      <c r="H61">
-        <f t="shared" si="25"/>
-        <v>0.65941461347624208</v>
-      </c>
-    </row>
-    <row r="62" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C62">
+      <c r="H63">
+        <f t="shared" si="26"/>
+        <v>0.72093509224866581</v>
+      </c>
+    </row>
+    <row r="64" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C64">
         <v>20</v>
       </c>
-      <c r="D62">
-        <f t="shared" ref="D62:H62" si="26">+D31/25.4</f>
+      <c r="D64">
+        <f t="shared" ref="D64:H64" si="27">+D31/25.4</f>
         <v>0.7331144819703318</v>
       </c>
-      <c r="E62">
-        <f t="shared" si="26"/>
+      <c r="E64">
+        <f t="shared" si="27"/>
         <v>0.73122925561757168</v>
       </c>
-      <c r="F62">
-        <f t="shared" si="26"/>
+      <c r="F64">
+        <f t="shared" si="27"/>
         <v>0.72835015779067047</v>
       </c>
-      <c r="G62">
-        <f t="shared" si="26"/>
+      <c r="G64">
+        <f t="shared" si="27"/>
         <v>0.72468728443323538</v>
       </c>
-      <c r="H62">
-        <f t="shared" si="26"/>
-        <v>0.63624765632876557</v>
-      </c>
-    </row>
-    <row r="63" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C63">
+      <c r="H64">
+        <f t="shared" si="27"/>
+        <v>0.71350182405596541</v>
+      </c>
+    </row>
+    <row r="65" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C65">
         <v>25</v>
       </c>
-      <c r="D63">
-        <f t="shared" ref="D63:H63" si="27">+D32/25.4</f>
+      <c r="D65">
+        <f t="shared" ref="D65:H65" si="28">+D32/25.4</f>
         <v>0.72994235550458131</v>
       </c>
-      <c r="E63">
-        <f t="shared" si="27"/>
+      <c r="E65">
+        <f t="shared" si="28"/>
         <v>0.72770296907233667</v>
       </c>
-      <c r="F63">
-        <f t="shared" si="27"/>
+      <c r="F65">
+        <f t="shared" si="28"/>
         <v>0.7242830017027807</v>
       </c>
-      <c r="G63">
-        <f t="shared" si="27"/>
+      <c r="G65">
+        <f t="shared" si="28"/>
         <v>0.71993201812584295</v>
       </c>
-      <c r="H63">
-        <f t="shared" si="27"/>
-        <v>0.61487805314178123</v>
-      </c>
-    </row>
-    <row r="64" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C64">
+      <c r="H65">
+        <f t="shared" si="28"/>
+        <v>0.70664524851826083</v>
+      </c>
+    </row>
+    <row r="66" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C66">
         <v>30</v>
       </c>
-      <c r="D64">
-        <f t="shared" ref="D64:H64" si="28">+D33/25.4</f>
+      <c r="D66">
+        <f t="shared" ref="D66:H66" si="29">+D33/25.4</f>
         <v>0.72696392265787313</v>
       </c>
-      <c r="E64">
-        <f t="shared" si="28"/>
+      <c r="E66">
+        <f t="shared" si="29"/>
         <v>0.72439200155996564</v>
       </c>
-      <c r="F64">
-        <f t="shared" si="28"/>
+      <c r="F66">
+        <f t="shared" si="29"/>
         <v>0.7204641907519399</v>
       </c>
-      <c r="G64">
-        <f t="shared" si="28"/>
+      <c r="G66">
+        <f t="shared" si="29"/>
         <v>0.71546711374144867</v>
       </c>
-      <c r="H64">
-        <f t="shared" si="28"/>
-        <v>0.59481330202279525</v>
-      </c>
-    </row>
-    <row r="65" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C65">
+      <c r="H66">
+        <f t="shared" si="29"/>
+        <v>0.70020734321469569</v>
+      </c>
+    </row>
+    <row r="67" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C67">
         <v>35</v>
       </c>
-      <c r="D65">
-        <f t="shared" ref="D65:H65" si="29">+D34/25.4</f>
+      <c r="D67">
+        <f t="shared" ref="D67:H67" si="30">+D34/25.4</f>
         <v>0.72413553507543715</v>
       </c>
-      <c r="E65">
-        <f t="shared" si="29"/>
+      <c r="E67">
+        <f t="shared" si="30"/>
         <v>0.7212478314947619</v>
       </c>
-      <c r="F65">
-        <f t="shared" si="29"/>
+      <c r="F67">
+        <f t="shared" si="30"/>
         <v>0.71683776100551588</v>
       </c>
-      <c r="G65">
-        <f t="shared" si="29"/>
+      <c r="G67">
+        <f t="shared" si="30"/>
         <v>0.71122713897366363</v>
       </c>
-      <c r="H65">
-        <f t="shared" si="29"/>
-        <v>0.57575935794199073</v>
-      </c>
-    </row>
-    <row r="66" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C66">
+      <c r="H67">
+        <f t="shared" si="30"/>
+        <v>0.69409376189369065</v>
+      </c>
+    </row>
+    <row r="68" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C68">
         <v>40</v>
       </c>
-      <c r="D66">
-        <f t="shared" ref="D66:H66" si="30">+D35/25.4</f>
+      <c r="D68">
+        <f t="shared" ref="D68:H68" si="31">+D35/25.4</f>
         <v>0.72142845544552847</v>
       </c>
-      <c r="E66">
-        <f t="shared" si="30"/>
+      <c r="E68">
+        <f t="shared" si="31"/>
         <v>0.71823851311515308</v>
       </c>
-      <c r="F66">
-        <f t="shared" si="30"/>
+      <c r="F68">
+        <f t="shared" si="31"/>
         <v>0.71336686679115779</v>
       </c>
-      <c r="G66">
-        <f t="shared" si="30"/>
+      <c r="G68">
+        <f t="shared" si="31"/>
         <v>0.70716901433880996</v>
       </c>
-      <c r="H66">
-        <f t="shared" si="30"/>
-        <v>0.5575226268055381</v>
-      </c>
-    </row>
-    <row r="67" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C67">
+      <c r="H68">
+        <f t="shared" si="31"/>
+        <v>0.68824238863683695</v>
+      </c>
+    </row>
+    <row r="69" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C69">
         <v>45</v>
       </c>
-      <c r="D67">
-        <f t="shared" ref="D67:H67" si="31">+D36/25.4</f>
+      <c r="D69">
+        <f t="shared" ref="D69:H69" si="32">+D36/25.4</f>
         <v>0.71882247409659372</v>
       </c>
-      <c r="E67">
-        <f t="shared" si="31"/>
+      <c r="E69">
+        <f t="shared" si="32"/>
         <v>0.71534158038970852</v>
       </c>
-      <c r="F67">
-        <f t="shared" si="31"/>
+      <c r="F69">
+        <f t="shared" si="32"/>
         <v>0.71002559618839844</v>
       </c>
-      <c r="G67">
-        <f t="shared" si="31"/>
+      <c r="G69">
+        <f t="shared" si="32"/>
         <v>0.70326244395453297</v>
       </c>
-      <c r="H67">
-        <f t="shared" si="31"/>
-        <v>0.53996696250883114</v>
-      </c>
-    </row>
-    <row r="68" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C68">
+      <c r="H69">
+        <f t="shared" si="32"/>
+        <v>0.6826095400850084</v>
+      </c>
+    </row>
+    <row r="70" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C70">
         <v>50</v>
       </c>
-      <c r="D68">
-        <f t="shared" ref="D68:H68" si="32">+D37/25.4</f>
+      <c r="D70">
+        <f t="shared" ref="D70:H70" si="33">+D37/25.4</f>
         <v>0.71630268450143153</v>
       </c>
-      <c r="E68">
-        <f t="shared" si="32"/>
+      <c r="E70">
+        <f t="shared" si="33"/>
         <v>0.71254046251430836</v>
       </c>
-      <c r="F68">
-        <f t="shared" si="32"/>
+      <c r="F70">
+        <f t="shared" si="33"/>
         <v>0.70679483672694032</v>
       </c>
-      <c r="G68">
-        <f t="shared" si="32"/>
+      <c r="G70">
+        <f t="shared" si="33"/>
         <v>0.69948508176769519</v>
       </c>
-      <c r="H68">
-        <f t="shared" si="32"/>
-        <v>0.5229919445375445</v>
-      </c>
-    </row>
-    <row r="69" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C69">
+      <c r="H70">
+        <f t="shared" si="33"/>
+        <v>0.67716299566602212</v>
+      </c>
+    </row>
+    <row r="71" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C71">
         <v>55</v>
       </c>
-      <c r="D69">
-        <f t="shared" ref="D69:H69" si="33">+D38/25.4</f>
+      <c r="D71">
+        <f t="shared" ref="D71:H71" si="34">+D38/25.4</f>
         <v>0.7138576868735701</v>
       </c>
-      <c r="E69">
-        <f t="shared" si="33"/>
+      <c r="E71">
+        <f t="shared" si="34"/>
         <v>0.70982248694449812</v>
       </c>
-      <c r="F69">
-        <f t="shared" si="33"/>
+      <c r="F71">
+        <f t="shared" si="34"/>
         <v>0.70365997211974385</v>
       </c>
-      <c r="G69">
-        <f t="shared" si="33"/>
+      <c r="G71">
+        <f t="shared" si="34"/>
         <v>0.69581983860448704</v>
       </c>
-      <c r="H69">
-        <f t="shared" si="33"/>
-        <v>0.50652077617000202</v>
-      </c>
-    </row>
-    <row r="70" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C70">
+      <c r="H71">
+        <f t="shared" si="34"/>
+        <v>0.67187811465451641</v>
+      </c>
+    </row>
+    <row r="72" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C72">
         <v>60</v>
       </c>
-      <c r="D70">
-        <f t="shared" ref="D70:H70" si="34">+D39/25.4</f>
+      <c r="D72">
+        <f t="shared" ref="D72:H72" si="35">+D39/25.4</f>
         <v>0.71147851205598589</v>
       </c>
-      <c r="E70">
-        <f t="shared" si="34"/>
+      <c r="E72">
+        <f t="shared" si="35"/>
         <v>0.70717768313904084</v>
       </c>
-      <c r="F70">
-        <f t="shared" si="34"/>
+      <c r="F72">
+        <f t="shared" si="35"/>
         <v>0.70060950252215104</v>
       </c>
-      <c r="G70">
-        <f t="shared" si="34"/>
+      <c r="G72">
+        <f t="shared" si="35"/>
         <v>0.69225326899523332</v>
       </c>
-      <c r="H70">
-        <f t="shared" si="34"/>
-        <v>0.49049303505905228</v>
-      </c>
-    </row>
-    <row r="71" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C71">
+      <c r="H72">
+        <f t="shared" si="35"/>
+        <v>0.66673551014920973</v>
+      </c>
+    </row>
+    <row r="73" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C73">
         <v>65</v>
       </c>
-      <c r="D71">
-        <f t="shared" ref="D71:H71" si="35">+D40/25.4</f>
+      <c r="D73">
+        <f t="shared" ref="D73:H73" si="36">+D40/25.4</f>
         <v>0.7091579396763229</v>
       </c>
-      <c r="E71">
-        <f t="shared" si="35"/>
+      <c r="E73">
+        <f t="shared" si="36"/>
         <v>0.70459802458885346</v>
       </c>
-      <c r="F71">
-        <f t="shared" si="35"/>
+      <c r="F73">
+        <f t="shared" si="36"/>
         <v>0.6976341703015605</v>
       </c>
-      <c r="G71">
-        <f t="shared" si="35"/>
+      <c r="G73">
+        <f t="shared" si="36"/>
         <v>0.68877454903560342</v>
       </c>
-      <c r="H71">
-        <f t="shared" si="35"/>
-        <v>0.47486007986149215</v>
-      </c>
-    </row>
-    <row r="72" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C72">
+      <c r="H73">
+        <f t="shared" si="36"/>
+        <v>0.66171957526021241</v>
+      </c>
+    </row>
+    <row r="74" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C74">
         <v>70</v>
       </c>
-      <c r="D72">
-        <f t="shared" ref="D72:H72" si="36">+D41/25.4</f>
+      <c r="D74">
+        <f t="shared" ref="D74:H74" si="37">+D41/25.4</f>
         <v>0.70689004631766394</v>
       </c>
-      <c r="E72">
-        <f t="shared" si="36"/>
+      <c r="E74">
+        <f t="shared" si="37"/>
         <v>0.70207692654216047</v>
       </c>
-      <c r="F72">
-        <f t="shared" si="36"/>
+      <c r="F74">
+        <f t="shared" si="37"/>
         <v>0.69472638072256843</v>
       </c>
-      <c r="G72">
-        <f t="shared" si="36"/>
+      <c r="G74">
+        <f t="shared" si="37"/>
         <v>0.68537479905916643</v>
       </c>
-      <c r="H72">
-        <f t="shared" si="36"/>
-        <v>0.45958200640880831</v>
-      </c>
-    </row>
-    <row r="73" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C73">
+      <c r="H74">
+        <f t="shared" si="37"/>
+        <v>0.65681750647670167</v>
+      </c>
+    </row>
+    <row r="75" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C75">
         <v>75</v>
       </c>
-      <c r="D73">
-        <f t="shared" ref="D73:H73" si="37">+D42/25.4</f>
+      <c r="D75">
+        <f t="shared" ref="D75:H75" si="38">+D42/25.4</f>
         <v>0.70466989493238885</v>
       </c>
-      <c r="E73">
-        <f t="shared" si="37"/>
+      <c r="E75">
+        <f t="shared" si="38"/>
         <v>0.69960890074217796</v>
       </c>
-      <c r="F73">
-        <f t="shared" si="37"/>
+      <c r="F75">
+        <f t="shared" si="38"/>
         <v>0.69187980372756153</v>
       </c>
-      <c r="G73">
-        <f t="shared" si="37"/>
+      <c r="G75">
+        <f t="shared" si="38"/>
         <v>0.6820466180444128</v>
       </c>
-      <c r="H73">
-        <f t="shared" si="37"/>
-        <v>0.44462555538751064</v>
-      </c>
-    </row>
-    <row r="74" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C74">
+      <c r="H75">
+        <f t="shared" si="38"/>
+        <v>0.65201863233261048</v>
+      </c>
+    </row>
+    <row r="76" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C76">
         <v>80</v>
       </c>
-      <c r="D74">
-        <f t="shared" ref="D74:H74" si="38">+D43/25.4</f>
+      <c r="D76">
+        <f t="shared" ref="D76:H76" si="39">+D43/25.4</f>
         <v>0.70249331471882981</v>
       </c>
-      <c r="E74">
-        <f t="shared" si="38"/>
+      <c r="E76">
+        <f t="shared" si="39"/>
         <v>0.69718931072754009</v>
       </c>
-      <c r="F74">
-        <f t="shared" si="38"/>
+      <c r="F76">
+        <f t="shared" si="39"/>
         <v>0.68908909170458954</v>
       </c>
-      <c r="G74">
-        <f t="shared" si="38"/>
+      <c r="G76">
+        <f t="shared" si="39"/>
         <v>0.67878375363259724</v>
       </c>
-      <c r="H74">
-        <f t="shared" si="38"/>
-        <v>0.42996262943843538</v>
-      </c>
-    </row>
-    <row r="75" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C75">
+      <c r="H76">
+        <f t="shared" si="39"/>
+        <v>0.647313937608338</v>
+      </c>
+    </row>
+    <row r="77" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C77">
         <v>85</v>
       </c>
-      <c r="D75">
-        <f t="shared" ref="D75:H75" si="39">+D44/25.4</f>
+      <c r="D77">
+        <f t="shared" ref="D77:H77" si="40">+D44/25.4</f>
         <v>0.70035674101848722</v>
       </c>
-      <c r="E75">
-        <f t="shared" si="39"/>
+      <c r="E77">
+        <f t="shared" si="40"/>
         <v>0.6948141938544371</v>
       </c>
-      <c r="F75">
-        <f t="shared" si="39"/>
+      <c r="F77">
+        <f t="shared" si="40"/>
         <v>0.68634967421086812</v>
       </c>
-      <c r="G75">
-        <f t="shared" si="39"/>
+      <c r="G77">
+        <f t="shared" si="40"/>
         <v>0.67558086212111523</v>
       </c>
-      <c r="H75">
-        <f t="shared" si="39"/>
-        <v>0.41556921459541663</v>
-      </c>
-    </row>
-    <row r="76" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C76">
+      <c r="H77">
+        <f t="shared" si="40"/>
+        <v>0.64269571726736396</v>
+      </c>
+    </row>
+    <row r="78" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C78">
         <v>90</v>
       </c>
-      <c r="D76">
-        <f t="shared" ref="D76:H76" si="40">+D45/25.4</f>
+      <c r="D78">
+        <f t="shared" ref="D78:H78" si="41">+D45/25.4</f>
         <v>0.69825709624969323</v>
       </c>
-      <c r="E76">
-        <f t="shared" si="40"/>
+      <c r="E78">
+        <f t="shared" si="41"/>
         <v>0.69248012893681443</v>
       </c>
-      <c r="F76">
-        <f t="shared" si="40"/>
+      <c r="F78">
+        <f t="shared" si="41"/>
         <v>0.68365760531134345</v>
       </c>
-      <c r="G76">
-        <f t="shared" si="40"/>
+      <c r="G78">
+        <f t="shared" si="41"/>
         <v>0.67243332997372451</v>
       </c>
-      <c r="H76">
-        <f t="shared" si="40"/>
-        <v>0.40142457817338251</v>
-      </c>
-    </row>
-    <row r="77" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C77">
+      <c r="H78">
+        <f t="shared" si="41"/>
+        <v>0.6381573190934513</v>
+      </c>
+    </row>
+    <row r="79" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C79">
         <v>95</v>
       </c>
-      <c r="D77">
-        <f t="shared" ref="D77:H77" si="41">+D46/25.4</f>
+      <c r="D79">
+        <f t="shared" ref="D79:H79" si="42">+D46/25.4</f>
         <v>0.69619169963345828</v>
       </c>
-      <c r="E77">
-        <f t="shared" si="41"/>
+      <c r="E79">
+        <f t="shared" si="42"/>
         <v>0.69018413589333416</v>
       </c>
-      <c r="F77">
-        <f t="shared" si="41"/>
+      <c r="F79">
+        <f t="shared" si="42"/>
         <v>0.68100944783328421</v>
       </c>
-      <c r="G77">
-        <f t="shared" si="41"/>
+      <c r="G79">
+        <f t="shared" si="42"/>
         <v>0.66933713849251231</v>
       </c>
-      <c r="H77">
-        <f t="shared" si="41"/>
-        <v>0.38751066062021261</v>
-      </c>
-    </row>
-    <row r="78" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C78">
+      <c r="H79">
+        <f t="shared" si="42"/>
+        <v>0.63369294856237801</v>
+      </c>
+    </row>
+    <row r="80" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C80">
         <v>100</v>
       </c>
-      <c r="D78">
-        <f t="shared" ref="D78:H78" si="42">+D47/25.4</f>
+      <c r="D80">
+        <f t="shared" ref="D80:H80" si="43">+D47/25.4</f>
         <v>0.6941581975809713</v>
       </c>
-      <c r="E78">
-        <f t="shared" si="42"/>
+      <c r="E80">
+        <f t="shared" si="43"/>
         <v>0.68792359836281181</v>
       </c>
-      <c r="F78">
-        <f t="shared" si="42"/>
+      <c r="F80">
+        <f t="shared" si="43"/>
         <v>0.67840218411230513</v>
       </c>
-      <c r="G78">
-        <f t="shared" si="42"/>
+      <c r="G80">
+        <f t="shared" si="43"/>
         <v>0.66628875946329946</v>
       </c>
-      <c r="H78">
-        <f t="shared" si="42"/>
-        <v>0.37381160655955337</v>
+      <c r="H80">
+        <f t="shared" si="43"/>
+        <v>0.62929751837398695</v>
       </c>
     </row>
   </sheetData>
@@ -11281,16 +11397,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B5:F27"/>
   <sheetViews>
-    <sheetView topLeftCell="C7" workbookViewId="0">
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="E5" t="s">
         <v>48</v>
       </c>
@@ -11298,7 +11414,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="E6" t="s">
         <v>49</v>
       </c>
@@ -11306,7 +11422,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" t="s">
         <v>45</v>
       </c>
@@ -11317,7 +11433,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B11">
         <v>1</v>
       </c>
@@ -11330,7 +11446,7 @@
         <v>89.91</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B12">
         <v>2</v>
       </c>
@@ -11343,7 +11459,7 @@
         <v>88.2</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B13">
         <v>3</v>
       </c>
@@ -11356,7 +11472,7 @@
         <v>86.490000000000009</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B14">
         <v>4</v>
       </c>
@@ -11369,7 +11485,7 @@
         <v>84.78</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B15">
         <v>5</v>
       </c>
@@ -11382,7 +11498,7 @@
         <v>83.070000000000007</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B16">
         <v>7.5</v>
       </c>
@@ -11395,7 +11511,7 @@
         <v>78.795000000000002</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B17">
         <v>10</v>
       </c>
@@ -11408,7 +11524,7 @@
         <v>74.52000000000001</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B18">
         <v>12.5</v>
       </c>
@@ -11421,7 +11537,7 @@
         <v>70.245000000000005</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B19">
         <v>15</v>
       </c>
@@ -11434,7 +11550,7 @@
         <v>65.970000000000013</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B20">
         <v>17.5</v>
       </c>
@@ -11447,7 +11563,7 @@
         <v>61.695</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B21">
         <v>20</v>
       </c>
@@ -11460,7 +11576,7 @@
         <v>57.42</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B22">
         <v>22.5</v>
       </c>
@@ -11473,7 +11589,7 @@
         <v>53.145000000000003</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B23">
         <v>25</v>
       </c>
@@ -11486,7 +11602,7 @@
         <v>48.870000000000005</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B24">
         <v>27.5</v>
       </c>
@@ -11499,7 +11615,7 @@
         <v>44.595000000000006</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B25">
         <v>30</v>
       </c>
@@ -11512,7 +11628,7 @@
         <v>40.320000000000007</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B26">
         <v>32.5</v>
       </c>
@@ -11525,7 +11641,7 @@
         <v>36.045000000000009</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B27">
         <v>35</v>
       </c>
@@ -11545,21 +11661,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B14:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="T25" sqref="T25"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="C14" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="2:5" ht="18" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:5" ht="16.8" x14ac:dyDescent="0.75">
       <c r="B15" t="s">
         <v>50</v>
       </c>
@@ -11573,7 +11689,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B16">
         <v>5</v>
       </c>
@@ -11590,7 +11706,7 @@
         <v>0.99680000000000002</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B17">
         <v>10</v>
       </c>
@@ -11607,7 +11723,7 @@
         <v>1.0098</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B18">
         <v>15</v>
       </c>
@@ -11624,7 +11740,7 @@
         <v>1.0227999999999999</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B19">
         <v>20</v>
       </c>
@@ -11641,7 +11757,7 @@
         <v>1.0358000000000001</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B20">
         <v>25</v>
       </c>
@@ -11658,7 +11774,7 @@
         <v>1.0488</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B21">
         <v>30</v>
       </c>
@@ -11675,7 +11791,7 @@
         <v>1.0618000000000001</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B22">
         <v>35</v>
       </c>
@@ -11692,7 +11808,7 @@
         <v>1.0748</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B23">
         <v>40</v>
       </c>
@@ -11709,7 +11825,7 @@
         <v>1.0878000000000001</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B24">
         <v>45</v>
       </c>
@@ -11726,7 +11842,7 @@
         <v>1.1008</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B25">
         <v>50</v>
       </c>
@@ -11743,7 +11859,7 @@
         <v>1.1137999999999999</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B26">
         <v>55</v>
       </c>
@@ -11760,7 +11876,7 @@
         <v>1.1268</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B27">
         <v>60</v>
       </c>
@@ -11777,7 +11893,7 @@
         <v>1.1397999999999999</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B28">
         <v>65</v>
       </c>
@@ -11794,7 +11910,7 @@
         <v>1.1528</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B29">
         <v>70</v>
       </c>
@@ -11811,7 +11927,7 @@
         <v>1.1657999999999999</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B30">
         <v>75</v>
       </c>
@@ -11835,25 +11951,25 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:W30"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="H63" sqref="H63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.26171875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.578125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -11864,7 +11980,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -11875,7 +11991,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -11887,7 +12003,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -11898,7 +12014,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2" t="s">
         <v>19</v>
       </c>
@@ -11906,7 +12022,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2" t="s">
         <v>21</v>
       </c>
@@ -11914,7 +12030,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -11940,7 +12056,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -11965,7 +12081,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -11990,7 +12106,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
@@ -11998,7 +12114,7 @@
         <v>0.622</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
@@ -12012,7 +12128,7 @@
         <v>7800</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="2" t="s">
         <v>18</v>
       </c>
@@ -12026,7 +12142,7 @@
         <v>3580</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="2" t="s">
         <v>26</v>
       </c>
@@ -12034,7 +12150,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -12070,7 +12186,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -12105,7 +12221,7 @@
         <v>3.8715707098347597E-13</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -12139,7 +12255,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -12172,7 +12288,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="J20">
         <v>1.26E-2</v>
       </c>
@@ -12193,7 +12309,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -12224,7 +12340,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="B22">
         <f>+B12*B21</f>
         <v>2.5316005173738394</v>
@@ -12253,12 +12369,12 @@
         <v>2.598741713530793E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="B24">
         <f>+(1-(B12/B11)*B10)</f>
         <v>0.71438775510204078</v>
@@ -12271,7 +12387,7 @@
         <v>3.5000000000000003E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="B25">
         <f>+B22/B24</f>
         <v>3.5437344765410121</v>
@@ -12293,18 +12409,18 @@
         <v>3.6370558894898097E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="F27">
         <f>+E25*4.88243</f>
         <v>0.16897732444651484</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="B29">
         <f>E25^2/(2*H25)</f>
         <v>3.2039334874712205E-5</v>
@@ -12318,7 +12434,7 @@
         <v>1708373233.3326151</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="U30">
         <f>+U29/(365*24*60*60)</f>
         <v>54.172159859608549</v>

</xml_diff>